<commit_message>
Added extra columns to the Excel data file. VersionUp
</commit_message>
<xml_diff>
--- a/inst/extdata/PlotSymptoms_shiny.xlsx
+++ b/inst/extdata/PlotSymptoms_shiny.xlsx
@@ -1,9 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="Ta_delovni_zvezek" defaultThemeVersion="124226"/>
-  <workbookProtection lockStructure="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crt Ahlin\Documents\Dropbox\medplot_package\inst\extdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="60" yWindow="30" windowWidth="14550" windowHeight="8145"/>
   </bookViews>
@@ -14,7 +18,7 @@
   <definedNames>
     <definedName name="executablesDir">#REF!</definedName>
     <definedName name="patientsTable">patientTable[]</definedName>
-    <definedName name="symptoms" localSheetId="0">DATA!$A$1:$Q$10</definedName>
+    <definedName name="symptoms" localSheetId="0">DATA!$A$1:$R$10</definedName>
     <definedName name="workingDir">#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621" calcMode="manual"/>
@@ -50,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
   <si>
     <t>Patient</t>
   </si>
@@ -70,9 +74,6 @@
     <t>11.4.2012</t>
   </si>
   <si>
-    <t>Miha</t>
-  </si>
-  <si>
     <t>13.3.2012</t>
   </si>
   <si>
@@ -88,24 +89,6 @@
     <t>27.3.2012</t>
   </si>
   <si>
-    <t>Nina</t>
-  </si>
-  <si>
-    <t>Črt</t>
-  </si>
-  <si>
-    <t>Luka</t>
-  </si>
-  <si>
-    <t>Sanja</t>
-  </si>
-  <si>
-    <t>Anja</t>
-  </si>
-  <si>
-    <t>Mina</t>
-  </si>
-  <si>
     <t>Headache</t>
   </si>
   <si>
@@ -143,13 +126,103 @@
   </si>
   <si>
     <t>High temperature</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>CaseorControl</t>
+  </si>
+  <si>
+    <t>PersonID</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>Črt Novak</t>
+  </si>
+  <si>
+    <t>Luka Pesek</t>
+  </si>
+  <si>
+    <t>Miha Vrat</t>
+  </si>
+  <si>
+    <t>Sanja Raven</t>
+  </si>
+  <si>
+    <t>Anja Uranja</t>
+  </si>
+  <si>
+    <t>Nina Kumina</t>
+  </si>
+  <si>
+    <t>Mina Eko</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>Brane Kovac</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +236,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -198,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -210,11 +290,32 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -251,6 +352,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -260,19 +364,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patientTable" displayName="patientTable" ref="A1:A8" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:A8"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="Patient" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patientTable" displayName="patientTable" ref="A1:E9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E9"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="PersonID" dataDxfId="0"/>
+    <tableColumn id="2" name="Name" dataDxfId="1"/>
+    <tableColumn id="3" name="Age" dataDxfId="4"/>
+    <tableColumn id="4" name="Sex" dataDxfId="3"/>
+    <tableColumn id="5" name="CaseorControl" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Officeova tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pisarna">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -310,9 +418,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pisarna">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -347,7 +455,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -382,7 +490,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pisarna">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -557,533 +665,564 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="11" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="17" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="9.140625" style="2"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="13.7109375" style="2" customWidth="1"/>
+    <col min="4" max="12" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="18" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="23" width="9.140625" style="2"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
-      <c r="R1" s="6"/>
+      <c r="R1" s="5"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
       <c r="V1" s="6"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
-        <v>2</v>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K2" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L2" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M2" s="2">
         <v>6</v>
       </c>
       <c r="N2" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O2" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="P2" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
-        <v>3</v>
+      <c r="C3" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
       </c>
       <c r="E3" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H3" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I3" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J3" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K3" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L3" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M3" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N3" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O3" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="P3" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
-        <v>3</v>
+      <c r="C4" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D4" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I4" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J4" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K4" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L4" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M4" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N4" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O4" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
-        <v>2</v>
+      <c r="C5" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H5" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L5" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="M5" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N5" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O5" s="2">
+        <v>9</v>
+      </c>
+      <c r="P5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D6" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I6" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J6" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K6" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L6" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M6" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N6" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E7" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I7" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J7" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K7" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L7" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N7" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O7" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="P7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D8" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G8" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J8" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K8" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L8" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M8" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N8" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O8" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2">
+        <v>9</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9</v>
+      </c>
+      <c r="K9" s="2">
+        <v>9</v>
+      </c>
+      <c r="L9" s="2">
+        <v>9</v>
+      </c>
+      <c r="M9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2">
+        <v>4</v>
+      </c>
+      <c r="O9" s="2">
+        <v>3</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>4</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>6</v>
-      </c>
-      <c r="G9" s="2">
-        <v>8</v>
-      </c>
-      <c r="H9" s="2">
-        <v>9</v>
-      </c>
-      <c r="I9" s="2">
-        <v>9</v>
-      </c>
-      <c r="J9" s="2">
-        <v>9</v>
-      </c>
-      <c r="K9" s="2">
-        <v>9</v>
-      </c>
-      <c r="L9" s="2">
-        <v>5</v>
-      </c>
-      <c r="M9" s="2">
-        <v>4</v>
-      </c>
-      <c r="N9" s="2">
-        <v>3</v>
-      </c>
-      <c r="O9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2">
-        <v>2</v>
+      <c r="C10" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="D10" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H10" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I10" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J10" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K10" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L10" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M10" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N10" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O10" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="P10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="D11" s="2">
-        <v>2</v>
-      </c>
       <c r="E11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I11" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J11" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K11" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L11" s="2">
         <v>9</v>
@@ -1097,435 +1236,464 @@
       <c r="O11" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P11" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="2">
-        <v>3</v>
+      <c r="C12" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
       </c>
       <c r="E12" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G12" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I12" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J12" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K12" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L12" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M12" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N12" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O12" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="P12" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="2">
-        <v>3</v>
+      <c r="C13" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D13" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G13" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I13" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J13" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K13" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L13" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M13" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N13" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O13" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P13" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="2">
-        <v>3</v>
+      <c r="C14" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
       </c>
       <c r="E14" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G14" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H14" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I14" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J14" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K14" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L14" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M14" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N14" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O14" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="P14" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="2">
-        <v>3</v>
+      <c r="C15" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D15" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F15" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I15" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J15" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K15" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L15" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M15" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N15" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O15" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="2">
-        <v>3</v>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
       </c>
       <c r="E16" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I16" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J16" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K16" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L16" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M16" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N16" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O16" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="P16" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="2">
-        <v>3</v>
+      <c r="C17" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="D17" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F17" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G17" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H17" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I17" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J17" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K17" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L17" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M17" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N17" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O17" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P17" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3</v>
+        <v>34</v>
+      </c>
+      <c r="B18" s="10">
+        <v>40986</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="D18" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E18" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F18" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I18" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J18" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K18" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L18" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M18" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N18" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O18" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P18" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2">
-        <v>3</v>
+        <v>34</v>
+      </c>
+      <c r="B19" s="10">
+        <v>40987</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="D19" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F19" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G19" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I19" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J19" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K19" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L19" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M19" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N19" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O19" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="P19" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="2">
-        <v>3</v>
+        <v>34</v>
+      </c>
+      <c r="B20" s="10">
+        <v>40988</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="D20" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F20" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G20" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I20" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J20" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K20" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L20" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M20" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N20" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O20" s="2">
+        <v>9</v>
+      </c>
+      <c r="P20" s="2">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
-      <formula1>patientsTable</formula1>
+      <formula1>INDIRECT("patientTable[PersonID]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1536,59 +1704,173 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="List1"/>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2">
+        <v>56</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Changed data example to simplify development.
</commit_message>
<xml_diff>
--- a/inst/extdata/PlotSymptoms_shiny.xlsx
+++ b/inst/extdata/PlotSymptoms_shiny.xlsx
@@ -143,27 +143,6 @@
     <t>PersonID</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>006</t>
-  </si>
-  <si>
-    <t>007</t>
-  </si>
-  <si>
     <t>Črt Novak</t>
   </si>
   <si>
@@ -194,9 +173,6 @@
     <t>Control</t>
   </si>
   <si>
-    <t>008</t>
-  </si>
-  <si>
     <t>Brane Kovac</t>
   </si>
   <si>
@@ -216,6 +192,30 @@
   </si>
   <si>
     <t>T4</t>
+  </si>
+  <si>
+    <t>ID001</t>
+  </si>
+  <si>
+    <t>ID002</t>
+  </si>
+  <si>
+    <t>ID003</t>
+  </si>
+  <si>
+    <t>ID004</t>
+  </si>
+  <si>
+    <t>ID005</t>
+  </si>
+  <si>
+    <t>ID006</t>
+  </si>
+  <si>
+    <t>ID007</t>
+  </si>
+  <si>
+    <t>ID008</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>11</v>
@@ -742,13 +742,13 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -792,13 +792,13 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -842,13 +842,13 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -892,13 +892,13 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -942,13 +942,13 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2">
         <v>3</v>
@@ -992,13 +992,13 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2">
         <v>4</v>
@@ -1042,13 +1042,13 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
@@ -1092,13 +1092,13 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -1142,13 +1142,13 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
@@ -1192,13 +1192,13 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -1242,13 +1242,13 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
@@ -1292,13 +1292,13 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2">
         <v>3</v>
@@ -1342,13 +1342,13 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2">
         <v>3</v>
@@ -1442,13 +1442,13 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -1492,13 +1492,13 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
@@ -1542,13 +1542,13 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B18" s="10">
         <v>40986</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -1592,13 +1592,13 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B19" s="10">
         <v>40987</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D19" s="2">
         <v>3</v>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B20" s="10">
         <v>40988</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2">
         <v>3</v>
@@ -1707,7 +1707,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,33 +1736,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C2" s="2">
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C3" s="2">
         <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>0</v>
@@ -1770,16 +1770,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C4" s="2">
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>0</v>
@@ -1787,33 +1787,33 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C5" s="2">
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C6" s="2">
         <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>0</v>
@@ -1821,16 +1821,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C7" s="2">
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>0</v>
@@ -1838,16 +1838,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C8" s="2">
         <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>0</v>
@@ -1855,19 +1855,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2">
         <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Template fix column type.
</commit_message>
<xml_diff>
--- a/inst/extdata/PlotSymptoms_shiny.xlsx
+++ b/inst/extdata/PlotSymptoms_shiny.xlsx
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -296,6 +296,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -669,13 +673,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
     <col min="3" max="3" width="13.7109375" style="2" customWidth="1"/>
     <col min="4" max="12" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="18" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -687,7 +691,7 @@
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -744,7 +748,7 @@
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -794,7 +798,7 @@
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -844,7 +848,7 @@
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -894,7 +898,7 @@
       <c r="A5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -944,7 +948,7 @@
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -994,7 +998,7 @@
       <c r="A7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1044,7 +1048,7 @@
       <c r="A8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="12" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1094,7 +1098,7 @@
       <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1144,7 +1148,7 @@
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1194,7 +1198,7 @@
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1244,7 +1248,7 @@
       <c r="A12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1294,7 +1298,7 @@
       <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1344,7 +1348,7 @@
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1394,7 +1398,7 @@
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1444,7 +1448,7 @@
       <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1494,7 +1498,7 @@
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1595,7 +1599,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="10">
-        <v>40987</v>
+        <v>40991</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>42</v>
@@ -1645,7 +1649,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="10">
-        <v>40988</v>
+        <v>40993</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Another fix of overriding Excel automaticity.
</commit_message>
<xml_diff>
--- a/inst/extdata/PlotSymptoms_shiny.xlsx
+++ b/inst/extdata/PlotSymptoms_shiny.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>Patient</t>
   </si>
@@ -216,6 +216,15 @@
   </si>
   <si>
     <t>ID008</t>
+  </si>
+  <si>
+    <t>18.3.2012</t>
+  </si>
+  <si>
+    <t>23.3.2012</t>
+  </si>
+  <si>
+    <t>25.3.2012</t>
   </si>
 </sst>
 </file>
@@ -278,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -296,10 +305,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -678,8 +683,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="9"/>
     <col min="3" max="3" width="13.7109375" style="2" customWidth="1"/>
     <col min="4" max="12" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="18" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -688,10 +693,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -745,10 +750,10 @@
       <c r="W1" s="6"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -795,10 +800,10 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -845,10 +850,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -895,10 +900,10 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -945,10 +950,10 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -995,10 +1000,10 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1045,10 +1050,10 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1095,10 +1100,10 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1145,10 +1150,10 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1195,10 +1200,10 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1245,10 +1250,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1295,10 +1300,10 @@
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1345,10 +1350,10 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1395,10 +1400,10 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1445,10 +1450,10 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1495,10 +1500,10 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1545,11 +1550,11 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="10">
-        <v>40986</v>
+      <c r="B18" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>41</v>
@@ -1595,11 +1600,11 @@
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="10">
-        <v>40991</v>
+      <c r="B19" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>42</v>
@@ -1645,11 +1650,11 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="10">
-        <v>40993</v>
+      <c r="B20" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Template data now a little more variable.
</commit_message>
<xml_diff>
--- a/inst/extdata/PlotSymptoms_shiny.xlsx
+++ b/inst/extdata/PlotSymptoms_shiny.xlsx
@@ -679,7 +679,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,10 +823,10 @@
         <v>2</v>
       </c>
       <c r="H3" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J3" s="2">
         <v>2</v>
@@ -847,7 +847,7 @@
         <v>7</v>
       </c>
       <c r="P3" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -891,13 +891,13 @@
         <v>4</v>
       </c>
       <c r="N4" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O4" s="2">
         <v>9</v>
       </c>
       <c r="P4" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -914,22 +914,22 @@
         <v>2</v>
       </c>
       <c r="E5" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
         <v>5</v>
       </c>
       <c r="H5" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I5" s="2">
         <v>7</v>
       </c>
       <c r="J5" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K5" s="2">
         <v>3</v>
@@ -1032,10 +1032,10 @@
         <v>8</v>
       </c>
       <c r="K7" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L7" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M7" s="2">
         <v>3</v>
@@ -1044,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="O7" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P7" s="2">
         <v>6</v>
@@ -1073,10 +1073,10 @@
         <v>2</v>
       </c>
       <c r="H8" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I8" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J8" s="2">
         <v>8</v>
@@ -1091,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O8" s="2">
         <v>9</v>
@@ -1129,7 +1129,7 @@
         <v>9</v>
       </c>
       <c r="J9" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K9" s="2">
         <v>9</v>
@@ -1223,7 +1223,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I11" s="2">
         <v>6</v>
@@ -1244,7 +1244,7 @@
         <v>9</v>
       </c>
       <c r="O11" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="P11" s="2">
         <v>9</v>
@@ -1267,7 +1267,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2">
         <v>2</v>
@@ -1314,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2">
         <v>7</v>
@@ -1329,7 +1329,7 @@
         <v>5</v>
       </c>
       <c r="J13" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2">
         <v>2</v>
@@ -1367,13 +1367,13 @@
         <v>3</v>
       </c>
       <c r="F14" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
         <v>2</v>
       </c>
       <c r="H14" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
         <v>8</v>
@@ -1388,7 +1388,7 @@
         <v>6</v>
       </c>
       <c r="M14" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
         <v>6</v>
@@ -1464,7 +1464,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
         <v>5</v>
@@ -1497,7 +1497,7 @@
         <v>7</v>
       </c>
       <c r="P16" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1517,7 +1517,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
         <v>2</v>
@@ -1573,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I18" s="2">
         <v>5</v>
@@ -1685,7 +1685,7 @@
         <v>2</v>
       </c>
       <c r="L20" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M20" s="2">
         <v>4</v>

</xml_diff>

<commit_message>
Internationalized names of Excel template subjects.
</commit_message>
<xml_diff>
--- a/inst/extdata/PlotSymptoms_shiny.xlsx
+++ b/inst/extdata/PlotSymptoms_shiny.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="30" windowWidth="14550" windowHeight="8145"/>
+    <workbookView xWindow="60" yWindow="30" windowWidth="14550" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="symptoms" localSheetId="0">DATA!$A$1:$R$10</definedName>
     <definedName name="workingDir">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -143,27 +143,6 @@
     <t>PersonID</t>
   </si>
   <si>
-    <t>Črt Novak</t>
-  </si>
-  <si>
-    <t>Luka Pesek</t>
-  </si>
-  <si>
-    <t>Miha Vrat</t>
-  </si>
-  <si>
-    <t>Sanja Raven</t>
-  </si>
-  <si>
-    <t>Anja Uranja</t>
-  </si>
-  <si>
-    <t>Nina Kumina</t>
-  </si>
-  <si>
-    <t>Mina Eko</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -173,9 +152,6 @@
     <t>Control</t>
   </si>
   <si>
-    <t>Brane Kovac</t>
-  </si>
-  <si>
     <t>Measurement</t>
   </si>
   <si>
@@ -225,6 +201,30 @@
   </si>
   <si>
     <t>25.3.2012</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Steven Doe</t>
+  </si>
+  <si>
+    <t>Michael Doe</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>Sue Doe</t>
+  </si>
+  <si>
+    <t>Ellen Doe</t>
+  </si>
+  <si>
+    <t>Anne Smith</t>
+  </si>
+  <si>
+    <t>John Smith</t>
   </si>
 </sst>
 </file>
@@ -314,7 +314,6 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -327,6 +326,7 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -377,11 +377,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="patientTable" displayName="patientTable" ref="A1:E9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E9"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="PersonID" dataDxfId="0"/>
-    <tableColumn id="2" name="Name" dataDxfId="1"/>
-    <tableColumn id="3" name="Age" dataDxfId="4"/>
-    <tableColumn id="4" name="Sex" dataDxfId="3"/>
-    <tableColumn id="5" name="CaseorControl" dataDxfId="2"/>
+    <tableColumn id="1" name="PersonID" dataDxfId="4"/>
+    <tableColumn id="2" name="Name" dataDxfId="3"/>
+    <tableColumn id="3" name="Age" dataDxfId="2"/>
+    <tableColumn id="4" name="Sex" dataDxfId="1"/>
+    <tableColumn id="5" name="CaseorControl" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -677,7 +677,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
@@ -701,7 +701,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>11</v>
@@ -752,13 +752,13 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -802,13 +802,13 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2">
         <v>3</v>
@@ -852,13 +852,13 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -902,13 +902,13 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -952,13 +952,13 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -1002,13 +1002,13 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2">
         <v>4</v>
@@ -1052,13 +1052,13 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2">
         <v>3</v>
@@ -1102,13 +1102,13 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2">
         <v>2</v>
@@ -1152,13 +1152,13 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D10" s="2">
         <v>2</v>
@@ -1202,13 +1202,13 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
@@ -1302,13 +1302,13 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2">
         <v>3</v>
@@ -1352,13 +1352,13 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
@@ -1402,13 +1402,13 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2">
         <v>3</v>
@@ -1452,13 +1452,13 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D16" s="2">
         <v>3</v>
@@ -1502,13 +1502,13 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
@@ -1552,13 +1552,13 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D19" s="2">
         <v>3</v>
@@ -1652,13 +1652,13 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D20" s="2">
         <v>3</v>
@@ -1716,8 +1716,8 @@
   <sheetPr codeName="List1"/>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,33 +1746,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2">
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2">
         <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>0</v>
@@ -1780,16 +1780,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2">
         <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>0</v>
@@ -1797,33 +1797,33 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2">
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2">
         <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>0</v>
@@ -1831,16 +1831,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2">
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>0</v>
@@ -1848,16 +1848,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2">
         <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>0</v>
@@ -1865,19 +1865,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2">
         <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>